<commit_message>
ClickOnElectronicstest added ClickOnComputersTest added BatchExecution added
</commit_message>
<xml_diff>
--- a/DemoWebShop/src/test/resources/testData/TestScriptData.xlsx
+++ b/DemoWebShop/src/test/resources/testData/TestScriptData.xlsx
@@ -3,37 +3,34 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B2C3B0D7-1DA8-4E37-85C5-257BCF6A923F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\git\DemoWebShoprepo\DemoWebShop\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23089745-DE97-44CD-AB15-5202161B5AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5F0C81DA-EF12-4B09-9B68-D38C0316B9A8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{5F0C81DA-EF12-4B09-9B68-D38C0316B9A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Books" sheetId="4" r:id="rId2"/>
-    <sheet name="Shopping Cart" sheetId="2" r:id="rId3"/>
-    <sheet name="Register" sheetId="3" r:id="rId4"/>
+    <sheet name="Computers" sheetId="5" r:id="rId3"/>
+    <sheet name="Electronics" sheetId="6" r:id="rId4"/>
+    <sheet name="Shopping Cart" sheetId="2" r:id="rId5"/>
+    <sheet name="Register" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:R13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Expected Title</t>
   </si>
@@ -78,6 +75,15 @@
   </si>
   <si>
     <t>Demo Web Shop. Books</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Demo Web Shop. Computers</t>
+  </si>
+  <si>
+    <t>Demo Web Shop. Electronics</t>
   </si>
 </sst>
 </file>
@@ -107,7 +113,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,6 +129,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD49CDC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -185,13 +203,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -199,6 +219,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFD49CDC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -555,7 +580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C0C238-880E-4A12-B5CD-FF11CEB6CFC2}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -580,6 +605,62 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{910889BA-199E-42C9-B5E8-DEA661BBA16F}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7245CFE1-958F-40FA-844B-84A06C7B43B0}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{405C4EBB-32FB-484F-82E3-B643F85D879B}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -607,7 +688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354EA1E8-C7BB-4559-80E2-3B7A939765B2}">
   <dimension ref="A1:E2"/>
   <sheetViews>

</xml_diff>